<commit_message>
clean htmls and demo_data
</commit_message>
<xml_diff>
--- a/utils/demo_data/iscatterplot.xlsx
+++ b/utils/demo_data/iscatterplot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiqbal/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiqbal/flaski/utils/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D252859F-7667-E445-B497-5B3976816A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A4927B-5A65-1E4E-A1B8-F2C5515FA65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{7BC24129-9FB3-9F45-A9E2-B4DBF4D595BA}"/>
   </bookViews>
@@ -39,76 +39,76 @@
     <t>group</t>
   </si>
   <si>
-    <t>CtrlOE_REP1</t>
-  </si>
-  <si>
-    <t>CtrlOE_REP2</t>
-  </si>
-  <si>
-    <t>CtrlOE_REP3</t>
-  </si>
-  <si>
-    <t>PrrOE_REP1</t>
-  </si>
-  <si>
-    <t>PrrOE_REP2</t>
-  </si>
-  <si>
-    <t>PrrOE_REP3</t>
-  </si>
-  <si>
-    <t>RagKO_REP1</t>
-  </si>
-  <si>
-    <t>RagKO_REP2</t>
-  </si>
-  <si>
-    <t>RagKO_REP3</t>
-  </si>
-  <si>
-    <t>RagWT_REP1</t>
-  </si>
-  <si>
-    <t>RagWT_REP2</t>
-  </si>
-  <si>
-    <t>RagWT_REP3</t>
-  </si>
-  <si>
-    <t>siLuc_REP1</t>
-  </si>
-  <si>
-    <t>siLuc_REP2</t>
-  </si>
-  <si>
-    <t>siLuc_REP3</t>
-  </si>
-  <si>
-    <t>siPRR_REP3</t>
-  </si>
-  <si>
-    <t>siPRR_REP1</t>
-  </si>
-  <si>
-    <t>siPRR_REP2</t>
-  </si>
-  <si>
-    <t>CtrlOE</t>
-  </si>
-  <si>
-    <t>PrrOE</t>
-  </si>
-  <si>
-    <t>RagKO</t>
-  </si>
-  <si>
-    <t>RagWT</t>
-  </si>
-  <si>
-    <t>siLuc</t>
-  </si>
-  <si>
-    <t>siPRR</t>
+    <t>WT_1</t>
+  </si>
+  <si>
+    <t>Mut_1</t>
+  </si>
+  <si>
+    <t>WT_2</t>
+  </si>
+  <si>
+    <t>Mut_2</t>
+  </si>
+  <si>
+    <t>WT_3</t>
+  </si>
+  <si>
+    <t>Mut_3</t>
+  </si>
+  <si>
+    <t>WT_1_Rep1</t>
+  </si>
+  <si>
+    <t>WT_1_Rep2</t>
+  </si>
+  <si>
+    <t>WT_1_Rep3</t>
+  </si>
+  <si>
+    <t>Mut_1_Rep1</t>
+  </si>
+  <si>
+    <t>Mut_1_Rep2</t>
+  </si>
+  <si>
+    <t>Mut_1_Rep3</t>
+  </si>
+  <si>
+    <t>WT_2_Rep1</t>
+  </si>
+  <si>
+    <t>WT_2_Rep2</t>
+  </si>
+  <si>
+    <t>WT_2_Rep3</t>
+  </si>
+  <si>
+    <t>Mut_2_Rep1</t>
+  </si>
+  <si>
+    <t>Mut_2_Rep2</t>
+  </si>
+  <si>
+    <t>Mut_2_Rep3</t>
+  </si>
+  <si>
+    <t>WT_3_Rep1</t>
+  </si>
+  <si>
+    <t>WT_3_Rep2</t>
+  </si>
+  <si>
+    <t>WT_3_Rep3</t>
+  </si>
+  <si>
+    <t>Mut_3_Rep1</t>
+  </si>
+  <si>
+    <t>Mut_3_Rep2</t>
+  </si>
+  <si>
+    <t>Mut_3_Rep3</t>
   </si>
 </sst>
 </file>
@@ -469,12 +469,12 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A17" sqref="A17:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,7 +494,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>5159.1705979999997</v>
@@ -503,12 +503,12 @@
         <v>120.07880501895301</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>5047.4351989999996</v>
@@ -517,12 +517,12 @@
         <v>102.55348026178901</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>5013.0318770000003</v>
@@ -531,12 +531,12 @@
         <v>91.209814313563001</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>4788.36096</v>
@@ -545,12 +545,12 @@
         <v>102.632553495366</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>4126.240315</v>
@@ -559,12 +559,12 @@
         <v>131.81416030026</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>4706.0782419999996</v>
@@ -573,12 +573,12 @@
         <v>115.022168222465</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>1663.328129</v>
@@ -587,12 +587,12 @@
         <v>3.6460892312356301</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>1687.461292</v>
@@ -601,12 +601,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1646.151016</v>
@@ -615,12 +615,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>6784.0702350000001</v>
@@ -629,12 +629,12 @@
         <v>62.499183293314402</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>6740.8758610000004</v>
@@ -643,12 +643,12 @@
         <v>80.092051360249798</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>6599.0811759999997</v>
@@ -657,12 +657,12 @@
         <v>80.172556181316494</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>4591.3654470000001</v>
@@ -671,12 +671,12 @@
         <v>65.295684396070399</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>4876.9753280000004</v>
@@ -685,12 +685,12 @@
         <v>63.702325714770801</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>4883.1461570000001</v>
@@ -699,12 +699,12 @@
         <v>79.309634552629603</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>4248.09933</v>
@@ -713,12 +713,12 @@
         <v>109.44168670956201</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>4281.6796459999996</v>
@@ -727,12 +727,12 @@
         <v>109.650630826662</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>3882.235514</v>
@@ -741,7 +741,7 @@
         <v>70.844478256185496</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>